<commit_message>
Releases y escenarios para planeamiento
</commit_message>
<xml_diff>
--- a/Gestion_Proyecto/Plan_Releases.xlsx
+++ b/Gestion_Proyecto/Plan_Releases.xlsx
@@ -1,21 +1,127 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PLANEAMIENTO" sheetId="1" r:id="rId1"/>
+    <sheet name="ESTRUCTURA_TRABAJO_US" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>ID_US</t>
+  </si>
+  <si>
+    <t>USER_STORY</t>
+  </si>
+  <si>
+    <t>DISCIPLINA</t>
+  </si>
+  <si>
+    <t>Requerimiento</t>
+  </si>
+  <si>
+    <t>Analisis</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Prueba Unitaria</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>TAREAS</t>
+  </si>
+  <si>
+    <t>Especificar UserStory &lt;ID&gt;</t>
+  </si>
+  <si>
+    <t>Diseñar Lógica de Aplicación</t>
+  </si>
+  <si>
+    <t>Diseñar Tablas</t>
+  </si>
+  <si>
+    <t>LINEAMIENTOS</t>
+  </si>
+  <si>
+    <t>PASOS A SEGUIR</t>
+  </si>
+  <si>
+    <t>1. Diseñar las tablas requeridas para soportar las necesidades de información de la User Story (/implementacion/worklist/worklist-dac / src / main / resources / db / migration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nota 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Se debe revisar si las tablas en la BD ya existen así como los campos de datos y relaciones con otras tablas. 
+Se debe colocar en archivo con extensión </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.sql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> siguiente el formato para su nombrado siguiente.
+a) Para crear o modificar la estructura de la base de datos se deberá utilizar:
+V4_(consecutivo)_Create_TaskManager_Schema.sql
+b) Si se colocarán registros como ejemplos en las tablas se deberá utilizar:
+V4_(consecutivo)_Fill_TaskManager_Default.sql</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Se debe actualizar el Diccionario de Datos con los cambios introducidos.</t>
+  </si>
+  <si>
+    <t>El archivo se encuentra ubicado en / Diseno / Diccionario_Datos.docx</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,13 +129,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -44,19 +172,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +489,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="71" style="2" customWidth="1"/>
+    <col min="5" max="5" width="63.28515625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>